<commit_message>
Local train loss: 0.29, val loss : 0.32 not uploaded:
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -382,1866 +382,1866 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>0.0002434963010076322</v>
+        <v>0.002590812557503027</v>
       </c>
       <c r="B2">
-        <v>0.9997565036989923</v>
+        <v>0.997409187442497</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>0.1303265963787791</v>
+        <v>0.2961098999981138</v>
       </c>
       <c r="B3">
-        <v>0.869673403621221</v>
+        <v>0.7038901000018861</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>0.8102968180198112</v>
+        <v>0.663527563210501</v>
       </c>
       <c r="B4">
-        <v>0.1897031819801887</v>
+        <v>0.336472436789499</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>0.0002143632184193593</v>
+        <v>0.00476154464118325</v>
       </c>
       <c r="B5">
-        <v>0.9997856367815807</v>
+        <v>0.9952384553588166</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>0.4294271799802554</v>
+        <v>0.398451998699122</v>
       </c>
       <c r="B6">
-        <v>0.5705728200197446</v>
+        <v>0.601548001300878</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>0.9303684820520531</v>
+        <v>0.6460110409111197</v>
       </c>
       <c r="B7">
-        <v>0.06963151794794699</v>
+        <v>0.3539889590888801</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>0.8200614942346285</v>
+        <v>0.742508921247145</v>
       </c>
       <c r="B8">
-        <v>0.1799385057653714</v>
+        <v>0.2574910787528552</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>0.9657946270353183</v>
+        <v>0.850922884269649</v>
       </c>
       <c r="B9">
-        <v>0.03420537296468173</v>
+        <v>0.1490771157303509</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>0.001006447295673925</v>
+        <v>0.02360250528078069</v>
       </c>
       <c r="B10">
-        <v>0.9989935527043259</v>
+        <v>0.9763974947192192</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>0.001051798125763992</v>
+        <v>0.01220786208729949</v>
       </c>
       <c r="B11">
-        <v>0.9989482018742361</v>
+        <v>0.9877921379127006</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>0.01540582339614328</v>
+        <v>0.04321889005179715</v>
       </c>
       <c r="B12">
-        <v>0.9845941766038567</v>
+        <v>0.9567811099482029</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>0.9444611871312412</v>
+        <v>0.8588827350961352</v>
       </c>
       <c r="B13">
-        <v>0.05553881286875873</v>
+        <v>0.1411172649038649</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>0.7275185127729766</v>
+        <v>0.4488096279818531</v>
       </c>
       <c r="B14">
-        <v>0.2724814872270233</v>
+        <v>0.5511903720181468</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>0.6985862695488352</v>
+        <v>0.5381287818690833</v>
       </c>
       <c r="B15">
-        <v>0.3014137304511648</v>
+        <v>0.4618712181309167</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>0.0001378554266758073</v>
+        <v>0.0141637610495182</v>
       </c>
       <c r="B16">
-        <v>0.9998621445733242</v>
+        <v>0.9858362389504817</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>0.9727781693511584</v>
+        <v>0.8221532667474605</v>
       </c>
       <c r="B17">
-        <v>0.02722183064884153</v>
+        <v>0.1778467332525395</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>0.5493637443645931</v>
+        <v>0.514903875079726</v>
       </c>
       <c r="B18">
-        <v>0.450636255635407</v>
+        <v>0.485096124920274</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>0.6795420029818536</v>
+        <v>0.4126876791528929</v>
       </c>
       <c r="B19">
-        <v>0.3204579970181465</v>
+        <v>0.5873123208471072</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>0.1088201313361358</v>
+        <v>0.06464216865605026</v>
       </c>
       <c r="B20">
-        <v>0.8911798686638641</v>
+        <v>0.9353578313439498</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>7.048576484209867E-05</v>
+        <v>0.001701629327904904</v>
       </c>
       <c r="B21">
-        <v>0.9999295142351577</v>
+        <v>0.9982983706720951</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>0.8334906370240612</v>
+        <v>0.6331309524642089</v>
       </c>
       <c r="B22">
-        <v>0.1665093629759389</v>
+        <v>0.366869047535791</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>0.7132286103541055</v>
+        <v>0.3713127900190087</v>
       </c>
       <c r="B23">
-        <v>0.2867713896458945</v>
+        <v>0.6286872099809914</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>0.08723051605157502</v>
+        <v>0.3309419741519523</v>
       </c>
       <c r="B24">
-        <v>0.9127694839484249</v>
+        <v>0.6690580258480476</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>0.9571864131552971</v>
+        <v>0.9232090623978889</v>
       </c>
       <c r="B25">
-        <v>0.04281358684470293</v>
+        <v>0.07679093760211116</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>0.9139332774845841</v>
+        <v>0.7323956862780158</v>
       </c>
       <c r="B26">
-        <v>0.08606672251541587</v>
+        <v>0.2676043137219845</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>0.0002578631734010036</v>
+        <v>0.008458869919169547</v>
       </c>
       <c r="B27">
-        <v>0.9997421368265988</v>
+        <v>0.9915411300808302</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>0.5405454329028601</v>
+        <v>0.4690468282515542</v>
       </c>
       <c r="B28">
-        <v>0.4594545670971399</v>
+        <v>0.5309531717484458</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>1.412675433483853E-05</v>
+        <v>0.0007412209456209018</v>
       </c>
       <c r="B29">
-        <v>0.9999858732456652</v>
+        <v>0.999258779054379</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>0.001376388891593031</v>
+        <v>0.02131428114060944</v>
       </c>
       <c r="B30">
-        <v>0.9986236111084071</v>
+        <v>0.9786857188593905</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>0.925515754706283</v>
+        <v>0.8855794020913983</v>
       </c>
       <c r="B31">
-        <v>0.07448424529371696</v>
+        <v>0.1144205979086017</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>0.8325374549162088</v>
+        <v>0.6920290719051596</v>
       </c>
       <c r="B32">
-        <v>0.1674625450837912</v>
+        <v>0.3079709280948403</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>0.001449901633852568</v>
+        <v>0.01934906934302971</v>
       </c>
       <c r="B33">
-        <v>0.9985500983661474</v>
+        <v>0.9806509306569704</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
-        <v>0.02950052177799011</v>
+        <v>0.04868653033919248</v>
       </c>
       <c r="B34">
-        <v>0.9704994782220099</v>
+        <v>0.9513134696608074</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>6.955896688128534E-05</v>
+        <v>0.001066210096426201</v>
       </c>
       <c r="B35">
-        <v>0.9999304410331187</v>
+        <v>0.9989337899035738</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>0.8886013902194347</v>
+        <v>0.6832424629037621</v>
       </c>
       <c r="B36">
-        <v>0.1113986097805652</v>
+        <v>0.3167575370962379</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>0.9683913921586472</v>
+        <v>0.8543998471527856</v>
       </c>
       <c r="B37">
-        <v>0.03160860784135271</v>
+        <v>0.1456001528472144</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38">
-        <v>1.154487171519669E-05</v>
+        <v>0.00103063586318423</v>
       </c>
       <c r="B38">
-        <v>0.9999884551282847</v>
+        <v>0.9989693641368158</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39">
-        <v>0.8640737048201372</v>
+        <v>0.7767970250585622</v>
       </c>
       <c r="B39">
-        <v>0.1359262951798627</v>
+        <v>0.2232029749414378</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40">
-        <v>0.8971824787652156</v>
+        <v>0.8275280027291133</v>
       </c>
       <c r="B40">
-        <v>0.1028175212347842</v>
+        <v>0.1724719972708866</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41">
-        <v>0.9501450400677981</v>
+        <v>0.7909627768694917</v>
       </c>
       <c r="B41">
-        <v>0.04985495993220208</v>
+        <v>0.2090372231305084</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42">
-        <v>0.001168821505606088</v>
+        <v>0.02636708730558874</v>
       </c>
       <c r="B42">
-        <v>0.998831178494394</v>
+        <v>0.9736329126944113</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43">
-        <v>0.9669489463663721</v>
+        <v>0.6927212729613571</v>
       </c>
       <c r="B43">
-        <v>0.03305105363362803</v>
+        <v>0.3072787270386428</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44">
-        <v>0.738541017994897</v>
+        <v>0.43531087566325</v>
       </c>
       <c r="B44">
-        <v>0.2614589820051031</v>
+        <v>0.56468912433675</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45">
-        <v>0.8775109648994747</v>
+        <v>0.6288924232004437</v>
       </c>
       <c r="B45">
-        <v>0.1224890351005253</v>
+        <v>0.3711075767995562</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46">
-        <v>0.0001745789281418109</v>
+        <v>0.001959313437407776</v>
       </c>
       <c r="B46">
-        <v>0.9998254210718581</v>
+        <v>0.9980406865625923</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47">
-        <v>0.8392664555770419</v>
+        <v>0.5597428669104654</v>
       </c>
       <c r="B47">
-        <v>0.160733544422958</v>
+        <v>0.4402571330895346</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48">
-        <v>0.9028755236895176</v>
+        <v>0.6252277911431012</v>
       </c>
       <c r="B48">
-        <v>0.09712447631048253</v>
+        <v>0.3747722088568988</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49">
-        <v>3.248289487907119E-05</v>
+        <v>0.0006229617456471548</v>
       </c>
       <c r="B49">
-        <v>0.999967517105121</v>
+        <v>0.9993770382543529</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50">
-        <v>0.02917159097424551</v>
+        <v>0.04851474348036501</v>
       </c>
       <c r="B50">
-        <v>0.9708284090257544</v>
+        <v>0.9514852565196349</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51">
-        <v>0.09088571990439911</v>
+        <v>0.2785993415916615</v>
       </c>
       <c r="B51">
-        <v>0.9091142800956009</v>
+        <v>0.7214006584083384</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52">
-        <v>0.2469582621476333</v>
+        <v>0.3016010153704168</v>
       </c>
       <c r="B52">
-        <v>0.7530417378523667</v>
+        <v>0.6983989846295832</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53">
-        <v>0.03295867005629285</v>
+        <v>0.03387900147435963</v>
       </c>
       <c r="B53">
-        <v>0.9670413299437073</v>
+        <v>0.9661209985256404</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54">
-        <v>0.9668876007889076</v>
+        <v>0.7876639588813312</v>
       </c>
       <c r="B54">
-        <v>0.03311239921109234</v>
+        <v>0.2123360411186688</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55">
-        <v>0.004008131486019736</v>
+        <v>0.04378216898041284</v>
       </c>
       <c r="B55">
-        <v>0.9959918685139802</v>
+        <v>0.9562178310195873</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56">
-        <v>0.4656620596514925</v>
+        <v>0.2552023908413459</v>
       </c>
       <c r="B56">
-        <v>0.5343379403485075</v>
+        <v>0.7447976091586541</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57">
-        <v>0.7520161985799535</v>
+        <v>0.468719310983933</v>
       </c>
       <c r="B57">
-        <v>0.2479838014200464</v>
+        <v>0.5312806890160668</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58">
-        <v>0.000107842538947948</v>
+        <v>0.00205905836998818</v>
       </c>
       <c r="B58">
-        <v>0.999892157461052</v>
+        <v>0.9979409416300119</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59">
-        <v>0.8389638789316862</v>
+        <v>0.7136785574887627</v>
       </c>
       <c r="B59">
-        <v>0.1610361210683136</v>
+        <v>0.2863214425112372</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60">
-        <v>0.9284519614192627</v>
+        <v>0.7117334786189282</v>
       </c>
       <c r="B60">
-        <v>0.07154803858073745</v>
+        <v>0.2882665213810718</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61">
-        <v>0.5077831354440809</v>
+        <v>0.1729095535964272</v>
       </c>
       <c r="B61">
-        <v>0.4922168645559192</v>
+        <v>0.8270904464035727</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62">
-        <v>0.980736767540345</v>
+        <v>0.878020559129716</v>
       </c>
       <c r="B62">
-        <v>0.01926323245965501</v>
+        <v>0.121979440870284</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63">
-        <v>0.8800156583757129</v>
+        <v>0.7603611691566112</v>
       </c>
       <c r="B63">
-        <v>0.1199843416242871</v>
+        <v>0.2396388308433887</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64">
-        <v>0.5090062289699401</v>
+        <v>0.1403998638822483</v>
       </c>
       <c r="B64">
-        <v>0.4909937710300599</v>
+        <v>0.8596001361177517</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65">
-        <v>0.01494448688094775</v>
+        <v>0.2235826217871664</v>
       </c>
       <c r="B65">
-        <v>0.9850555131190523</v>
+        <v>0.7764173782128335</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66">
-        <v>0.7508092247517921</v>
+        <v>0.5519814470004765</v>
       </c>
       <c r="B66">
-        <v>0.2491907752482079</v>
+        <v>0.4480185529995235</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67">
-        <v>0.8517288396661247</v>
+        <v>0.5437010513940181</v>
       </c>
       <c r="B67">
-        <v>0.1482711603338753</v>
+        <v>0.4562989486059819</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68">
-        <v>0.001171346196867459</v>
+        <v>0.009124588552720655</v>
       </c>
       <c r="B68">
-        <v>0.9988286538031325</v>
+        <v>0.9908754114472792</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69">
-        <v>0.9039006917432005</v>
+        <v>0.7899445828938207</v>
       </c>
       <c r="B69">
-        <v>0.09609930825679941</v>
+        <v>0.2100554171061792</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70">
-        <v>0.5155013457215221</v>
+        <v>0.2362239917412662</v>
       </c>
       <c r="B70">
-        <v>0.4844986542784779</v>
+        <v>0.7637760082587339</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71">
-        <v>0.8556375430562324</v>
+        <v>0.6463657618386142</v>
       </c>
       <c r="B71">
-        <v>0.1443624569437678</v>
+        <v>0.3536342381613859</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72">
-        <v>0.5958775680788621</v>
+        <v>0.5808074426767711</v>
       </c>
       <c r="B72">
-        <v>0.4041224319211379</v>
+        <v>0.419192557323229</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73">
-        <v>0.0004858364119946742</v>
+        <v>0.0009024998518503505</v>
       </c>
       <c r="B73">
-        <v>0.9995141635880054</v>
+        <v>0.9990975001481496</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74">
-        <v>0.005076801071241377</v>
+        <v>0.009959005844862801</v>
       </c>
       <c r="B74">
-        <v>0.9949231989287589</v>
+        <v>0.9900409941551371</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75">
-        <v>5.466697536026614E-05</v>
+        <v>0.0008863199936380999</v>
       </c>
       <c r="B75">
-        <v>0.9999453330246396</v>
+        <v>0.9991136800063618</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76">
-        <v>0.5748469901361002</v>
+        <v>0.3212612993806395</v>
       </c>
       <c r="B76">
-        <v>0.4251530098638999</v>
+        <v>0.6787387006193605</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77">
-        <v>0.0019112906768831</v>
+        <v>0.009508694925771369</v>
       </c>
       <c r="B77">
-        <v>0.9980887093231169</v>
+        <v>0.9904913050742288</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78">
-        <v>0.6407835611994706</v>
+        <v>0.4738531767303711</v>
       </c>
       <c r="B78">
-        <v>0.3592164388005293</v>
+        <v>0.5261468232696287</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79">
-        <v>0.002614382631760356</v>
+        <v>0.003808310730531613</v>
       </c>
       <c r="B79">
-        <v>0.9973856173682397</v>
+        <v>0.9961916892694682</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80">
-        <v>0.8173270674450038</v>
+        <v>0.5659603917004732</v>
       </c>
       <c r="B80">
-        <v>0.1826729325549962</v>
+        <v>0.4340396082995268</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81">
-        <v>0.001257642094663266</v>
+        <v>0.009810007470646398</v>
       </c>
       <c r="B81">
-        <v>0.9987423579053368</v>
+        <v>0.9901899925293536</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82">
-        <v>0.000122148783124317</v>
+        <v>0.0006759827005721124</v>
       </c>
       <c r="B82">
-        <v>0.9998778512168756</v>
+        <v>0.9993240172994278</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83">
-        <v>0.1448233523852429</v>
+        <v>0.2377673209753183</v>
       </c>
       <c r="B83">
-        <v>0.8551766476147571</v>
+        <v>0.7622326790246817</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84">
-        <v>0.4673291013301372</v>
+        <v>0.4267467998462292</v>
       </c>
       <c r="B84">
-        <v>0.5326708986698628</v>
+        <v>0.5732532001537708</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85">
-        <v>0.7851745610653679</v>
+        <v>0.774845233113815</v>
       </c>
       <c r="B85">
-        <v>0.2148254389346321</v>
+        <v>0.225154766886185</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86">
-        <v>0.9669044780041031</v>
+        <v>0.7671014288503615</v>
       </c>
       <c r="B86">
-        <v>0.03309552199589685</v>
+        <v>0.2328985711496384</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87">
-        <v>0.9533130221644943</v>
+        <v>0.9249464821194667</v>
       </c>
       <c r="B87">
-        <v>0.04668697783550566</v>
+        <v>0.07505351788053324</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88">
-        <v>0.001354054694837914</v>
+        <v>0.002022329040128904</v>
       </c>
       <c r="B88">
-        <v>0.998645945305162</v>
+        <v>0.9979776709598712</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89">
-        <v>0.1821399645203752</v>
+        <v>0.1945814419381248</v>
       </c>
       <c r="B89">
-        <v>0.8178600354796248</v>
+        <v>0.8054185580618752</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90">
-        <v>0.8501693790308305</v>
+        <v>0.6687589415762829</v>
       </c>
       <c r="B90">
-        <v>0.1498306209691696</v>
+        <v>0.331241058423717</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91">
-        <v>0.782396095527197</v>
+        <v>0.7665442300570452</v>
       </c>
       <c r="B91">
-        <v>0.217603904472803</v>
+        <v>0.2334557699429547</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92">
-        <v>0.6441085206359422</v>
+        <v>0.5085328407418132</v>
       </c>
       <c r="B92">
-        <v>0.3558914793640578</v>
+        <v>0.4914671592581869</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93">
-        <v>0.005657675069977771</v>
+        <v>0.083625515075608</v>
       </c>
       <c r="B93">
-        <v>0.9943423249300222</v>
+        <v>0.9163744849243918</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94">
-        <v>0.04455792971872725</v>
+        <v>0.07871527502264462</v>
       </c>
       <c r="B94">
-        <v>0.9554420702812727</v>
+        <v>0.9212847249773556</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95">
-        <v>0.9140423944070027</v>
+        <v>0.7765516832600661</v>
       </c>
       <c r="B95">
-        <v>0.08595760559299731</v>
+        <v>0.2234483167399342</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96">
-        <v>0.002316419715098705</v>
+        <v>0.005109621441824215</v>
       </c>
       <c r="B96">
-        <v>0.9976835802849013</v>
+        <v>0.9948903785581759</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97">
-        <v>0.0006911513639474398</v>
+        <v>0.006071504926609002</v>
       </c>
       <c r="B97">
-        <v>0.9993088486360524</v>
+        <v>0.9939284950733911</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98">
-        <v>0.9334730757489665</v>
+        <v>0.5965394025157755</v>
       </c>
       <c r="B98">
-        <v>0.06652692425103342</v>
+        <v>0.4034605974842245</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99">
-        <v>0.8103369451029011</v>
+        <v>0.5295407910576</v>
       </c>
       <c r="B99">
-        <v>0.189663054897099</v>
+        <v>0.4704592089424001</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100">
-        <v>0.6858047637848792</v>
+        <v>0.5886327975928914</v>
       </c>
       <c r="B100">
-        <v>0.314195236215121</v>
+        <v>0.4113672024071085</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101">
-        <v>0.0118739304603124</v>
+        <v>0.03252347816527927</v>
       </c>
       <c r="B101">
-        <v>0.9881260695396876</v>
+        <v>0.9674765218347205</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102">
-        <v>0.6339733920415555</v>
+        <v>0.4355087253500961</v>
       </c>
       <c r="B102">
-        <v>0.3660266079584445</v>
+        <v>0.5644912746499038</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103">
-        <v>0.8651004781959554</v>
+        <v>0.8109942870042665</v>
       </c>
       <c r="B103">
-        <v>0.1348995218040445</v>
+        <v>0.1890057129957336</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104">
-        <v>0.0001163143653847065</v>
+        <v>0.001514267255451814</v>
       </c>
       <c r="B104">
-        <v>0.9998836856346152</v>
+        <v>0.998485732744548</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105">
-        <v>0.4095337234683924</v>
+        <v>0.3076808199273238</v>
       </c>
       <c r="B105">
-        <v>0.5904662765316075</v>
+        <v>0.6923191800726763</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106">
-        <v>0.5138963456892185</v>
+        <v>0.5749832951361574</v>
       </c>
       <c r="B106">
-        <v>0.4861036543107815</v>
+        <v>0.4250167048638425</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107">
-        <v>2.055581830620786E-05</v>
+        <v>0.000588262384925442</v>
       </c>
       <c r="B107">
-        <v>0.9999794441816938</v>
+        <v>0.9994117376150746</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108">
-        <v>0.8567817792209627</v>
+        <v>0.5669722126966978</v>
       </c>
       <c r="B108">
-        <v>0.1432182207790373</v>
+        <v>0.4330277873033021</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109">
-        <v>1.401714077856238E-05</v>
+        <v>0.001119737329347581</v>
       </c>
       <c r="B109">
-        <v>0.9999859828592214</v>
+        <v>0.9988802626706524</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110">
-        <v>0.6113868846829484</v>
+        <v>0.4092669766575656</v>
       </c>
       <c r="B110">
-        <v>0.3886131153170517</v>
+        <v>0.5907330233424344</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111">
-        <v>6.018013404327505E-05</v>
+        <v>0.001228832615315115</v>
       </c>
       <c r="B111">
-        <v>0.9999398198659567</v>
+        <v>0.998771167384685</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112">
-        <v>0.9410789546287773</v>
+        <v>0.7759297157467985</v>
       </c>
       <c r="B112">
-        <v>0.05892104537122269</v>
+        <v>0.2240702842532015</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113">
-        <v>0.7792475633994038</v>
+        <v>0.4744786019015698</v>
       </c>
       <c r="B113">
-        <v>0.2207524366005961</v>
+        <v>0.52552139809843</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114">
-        <v>0.0218111654014174</v>
+        <v>0.03400757453859102</v>
       </c>
       <c r="B114">
-        <v>0.9781888345985826</v>
+        <v>0.965992425461409</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115">
-        <v>0.8004120844267061</v>
+        <v>0.6907844907695541</v>
       </c>
       <c r="B115">
-        <v>0.1995879155732938</v>
+        <v>0.3092155092304461</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116">
-        <v>0.6416940402540613</v>
+        <v>0.5799032957125896</v>
       </c>
       <c r="B116">
-        <v>0.3583059597459387</v>
+        <v>0.4200967042874106</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117">
-        <v>0.03185727489260528</v>
+        <v>0.1425547565239791</v>
       </c>
       <c r="B117">
-        <v>0.9681427251073949</v>
+        <v>0.8574452434760208</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118">
-        <v>0.0001659265021205059</v>
+        <v>0.0006963264615153619</v>
       </c>
       <c r="B118">
-        <v>0.9998340734978796</v>
+        <v>0.9993036735384848</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119">
-        <v>0.04578342099638341</v>
+        <v>0.1572712088348775</v>
       </c>
       <c r="B119">
-        <v>0.9542165790036167</v>
+        <v>0.8427287911651226</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120">
-        <v>0.001357054106022715</v>
+        <v>0.03479643780649599</v>
       </c>
       <c r="B120">
-        <v>0.9986429458939772</v>
+        <v>0.9652035621935039</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121">
-        <v>4.066314050498547E-05</v>
+        <v>0.001203812000249919</v>
       </c>
       <c r="B121">
-        <v>0.999959336859495</v>
+        <v>0.9987961879997499</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122">
-        <v>0.6162388054798729</v>
+        <v>0.4530384306837048</v>
       </c>
       <c r="B122">
-        <v>0.3837611945201271</v>
+        <v>0.5469615693162952</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123">
-        <v>0.0005675050635736886</v>
+        <v>0.004751896368102493</v>
       </c>
       <c r="B123">
-        <v>0.9994324949364262</v>
+        <v>0.9952481036318975</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124">
-        <v>0.9360140273959552</v>
+        <v>0.8798493411556078</v>
       </c>
       <c r="B124">
-        <v>0.0639859726040448</v>
+        <v>0.1201506588443922</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125">
-        <v>0.9579560064381927</v>
+        <v>0.8095122277133461</v>
       </c>
       <c r="B125">
-        <v>0.04204399356180723</v>
+        <v>0.1904877722866539</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126">
-        <v>0.7984311144595498</v>
+        <v>0.6341574993664624</v>
       </c>
       <c r="B126">
-        <v>0.2015688855404502</v>
+        <v>0.3658425006335377</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127">
-        <v>2.579281658639706E-05</v>
+        <v>0.0006561318421529776</v>
       </c>
       <c r="B127">
-        <v>0.9999742071834137</v>
+        <v>0.9993438681578469</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128">
-        <v>0.607974215931423</v>
+        <v>0.3469900355961011</v>
       </c>
       <c r="B128">
-        <v>0.3920257840685771</v>
+        <v>0.6530099644038987</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129">
-        <v>0.05040743440713858</v>
+        <v>0.08889688959209328</v>
       </c>
       <c r="B129">
-        <v>0.9495925655928613</v>
+        <v>0.9111031104079067</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130">
-        <v>0.1696294088631158</v>
+        <v>0.1948099081734133</v>
       </c>
       <c r="B130">
-        <v>0.8303705911368842</v>
+        <v>0.8051900918265866</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131">
-        <v>0.03644613743368871</v>
+        <v>0.03738446629762401</v>
       </c>
       <c r="B131">
-        <v>0.9635538625663113</v>
+        <v>0.9626155337023762</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132">
-        <v>0.8543684139917623</v>
+        <v>0.7904158233534154</v>
       </c>
       <c r="B132">
-        <v>0.1456315860082375</v>
+        <v>0.2095841766465846</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133">
-        <v>0.9456575026502514</v>
+        <v>0.7613240637978694</v>
       </c>
       <c r="B133">
-        <v>0.05434249734974852</v>
+        <v>0.2386759362021307</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134">
-        <v>0.9958971086122613</v>
+        <v>0.9611047494386956</v>
       </c>
       <c r="B134">
-        <v>0.004102891387738819</v>
+        <v>0.03889525056130426</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135">
-        <v>0.7820560518626071</v>
+        <v>0.6213391731258903</v>
       </c>
       <c r="B135">
-        <v>0.2179439481373929</v>
+        <v>0.3786608268741097</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136">
-        <v>0.0009312486662623077</v>
+        <v>0.004949604284314946</v>
       </c>
       <c r="B136">
-        <v>0.9990687513337378</v>
+        <v>0.995050395715685</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137">
-        <v>0.009176213904142397</v>
+        <v>0.03479812875665058</v>
       </c>
       <c r="B137">
-        <v>0.9908237860958575</v>
+        <v>0.9652018712433494</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138">
-        <v>0.04174388149225743</v>
+        <v>0.07509338137794448</v>
       </c>
       <c r="B138">
-        <v>0.9582561185077427</v>
+        <v>0.9249066186220556</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139">
-        <v>0.7061849588027561</v>
+        <v>0.4561876046703849</v>
       </c>
       <c r="B139">
-        <v>0.2938150411972439</v>
+        <v>0.543812395329615</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140">
-        <v>0.8880232526693731</v>
+        <v>0.7690596056496053</v>
       </c>
       <c r="B140">
-        <v>0.1119767473306268</v>
+        <v>0.2309403943503948</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141">
-        <v>0.6921852932555171</v>
+        <v>0.5481643633461737</v>
       </c>
       <c r="B141">
-        <v>0.3078147067444831</v>
+        <v>0.4518356366538265</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142">
-        <v>0.007361460452700045</v>
+        <v>0.01368796923828695</v>
       </c>
       <c r="B142">
-        <v>0.9926385395472999</v>
+        <v>0.9863120307617129</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143">
-        <v>0.6985311702560344</v>
+        <v>0.4952416361450793</v>
       </c>
       <c r="B143">
-        <v>0.3014688297439655</v>
+        <v>0.5047583638549206</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144">
-        <v>0.02539475467822015</v>
+        <v>0.05700901028761648</v>
       </c>
       <c r="B144">
-        <v>0.9746052453217797</v>
+        <v>0.9429909897123836</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145">
-        <v>0.05710896301702009</v>
+        <v>0.2840373887971593</v>
       </c>
       <c r="B145">
-        <v>0.9428910369829799</v>
+        <v>0.7159626112028407</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146">
-        <v>0.6803669932223897</v>
+        <v>0.6756353668572163</v>
       </c>
       <c r="B146">
-        <v>0.3196330067776102</v>
+        <v>0.3243646331427837</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147">
-        <v>0.03657461583007514</v>
+        <v>0.0704472043568337</v>
       </c>
       <c r="B147">
-        <v>0.963425384169925</v>
+        <v>0.9295527956431663</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148">
-        <v>0.0002199847103792063</v>
+        <v>0.0005456985886222565</v>
       </c>
       <c r="B148">
-        <v>0.9997800152896209</v>
+        <v>0.9994543014113775</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149">
-        <v>0.0001130784003118131</v>
+        <v>0.002363181306236265</v>
       </c>
       <c r="B149">
-        <v>0.9998869215996881</v>
+        <v>0.9976368186937636</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150">
-        <v>0.7943547184511381</v>
+        <v>0.4659526000419862</v>
       </c>
       <c r="B150">
-        <v>0.2056452815488619</v>
+        <v>0.5340473999580139</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151">
-        <v>0.8376328102822171</v>
+        <v>0.5353172942096829</v>
       </c>
       <c r="B151">
-        <v>0.162367189717783</v>
+        <v>0.4646827057903172</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152">
-        <v>0.0008185467960234894</v>
+        <v>0.002995361565081075</v>
       </c>
       <c r="B152">
-        <v>0.9991814532039766</v>
+        <v>0.997004638434919</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153">
-        <v>0.7527004040619415</v>
+        <v>0.6135243246666252</v>
       </c>
       <c r="B153">
-        <v>0.2472995959380586</v>
+        <v>0.3864756753333748</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154">
-        <v>0.7978095104121956</v>
+        <v>0.3966946541837307</v>
       </c>
       <c r="B154">
-        <v>0.2021904895878043</v>
+        <v>0.6033053458162694</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155">
-        <v>0.8861619725054718</v>
+        <v>0.658161176928902</v>
       </c>
       <c r="B155">
-        <v>0.1138380274945281</v>
+        <v>0.341838823071098</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156">
-        <v>0.5160474453852362</v>
+        <v>0.4336142931049014</v>
       </c>
       <c r="B156">
-        <v>0.4839525546147639</v>
+        <v>0.5663857068950986</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157">
-        <v>0.460385557604218</v>
+        <v>0.257522396451752</v>
       </c>
       <c r="B157">
-        <v>0.539614442395782</v>
+        <v>0.7424776035482481</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158">
-        <v>0.6503521906347682</v>
+        <v>0.5060218492154073</v>
       </c>
       <c r="B158">
-        <v>0.3496478093652317</v>
+        <v>0.4939781507845928</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159">
-        <v>0.002127946771528277</v>
+        <v>0.003112229431723801</v>
       </c>
       <c r="B159">
-        <v>0.9978720532284717</v>
+        <v>0.9968877705682762</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160">
-        <v>0.04409446960201557</v>
+        <v>0.2336565535799202</v>
       </c>
       <c r="B160">
-        <v>0.9559055303979844</v>
+        <v>0.7663434464200799</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161">
-        <v>0.001830666596851331</v>
+        <v>0.004954213260234345</v>
       </c>
       <c r="B161">
-        <v>0.9981693334031487</v>
+        <v>0.9950457867397656</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162">
-        <v>0.0003392328220352514</v>
+        <v>0.001034959681902466</v>
       </c>
       <c r="B162">
-        <v>0.9996607671779647</v>
+        <v>0.9989650403180976</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163">
-        <v>0.7728569486949687</v>
+        <v>0.6400848240299903</v>
       </c>
       <c r="B163">
-        <v>0.2271430513050313</v>
+        <v>0.3599151759700096</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164">
-        <v>0.9872294692667529</v>
+        <v>0.9096153970464155</v>
       </c>
       <c r="B164">
-        <v>0.01277053073324722</v>
+        <v>0.09038460295358459</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165">
-        <v>0.5625854456690947</v>
+        <v>0.2413494880935339</v>
       </c>
       <c r="B165">
-        <v>0.4374145543309051</v>
+        <v>0.7586505119064662</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166">
-        <v>0.03399104610244798</v>
+        <v>0.04914030473778152</v>
       </c>
       <c r="B166">
-        <v>0.966008953897552</v>
+        <v>0.9508596952622186</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167">
-        <v>0.4964890045669971</v>
+        <v>0.4172344587377958</v>
       </c>
       <c r="B167">
-        <v>0.5035109954330029</v>
+        <v>0.582765541262204</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168">
-        <v>0.7764914849844069</v>
+        <v>0.3486599168647192</v>
       </c>
       <c r="B168">
-        <v>0.2235085150155932</v>
+        <v>0.6513400831352809</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169">
-        <v>0.01979316066193256</v>
+        <v>0.0494135615771493</v>
       </c>
       <c r="B169">
-        <v>0.9802068393380676</v>
+        <v>0.9505864384228506</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170">
-        <v>2.110320801849141E-05</v>
+        <v>0.001428448723904574</v>
       </c>
       <c r="B170">
-        <v>0.9999788967919815</v>
+        <v>0.9985715512760954</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171">
-        <v>0.7662686265541192</v>
+        <v>0.5263833587778897</v>
       </c>
       <c r="B171">
-        <v>0.2337313734458807</v>
+        <v>0.4736166412221103</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172">
-        <v>1.208616206879546E-05</v>
+        <v>0.0005991239487194821</v>
       </c>
       <c r="B172">
-        <v>0.9999879138379312</v>
+        <v>0.9994008760512804</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173">
-        <v>0.004205498700238526</v>
+        <v>0.03426089819071576</v>
       </c>
       <c r="B173">
-        <v>0.9957945012997614</v>
+        <v>0.9657391018092842</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174">
-        <v>8.200572027702671E-05</v>
+        <v>0.001334411591162328</v>
       </c>
       <c r="B174">
-        <v>0.9999179942797231</v>
+        <v>0.9986655884088377</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175">
-        <v>0.7223290128895623</v>
+        <v>0.6920377743422874</v>
       </c>
       <c r="B175">
-        <v>0.2776709871104376</v>
+        <v>0.3079622256577126</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176">
-        <v>0.8169258487178954</v>
+        <v>0.7316990341238169</v>
       </c>
       <c r="B176">
-        <v>0.1830741512821046</v>
+        <v>0.268300965876183</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177">
-        <v>0.002356485433363338</v>
+        <v>0.04629917033905275</v>
       </c>
       <c r="B177">
-        <v>0.9976435145666368</v>
+        <v>0.9537008296609473</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178">
-        <v>0.4817449648951006</v>
+        <v>0.1981204250002354</v>
       </c>
       <c r="B178">
-        <v>0.5182550351048995</v>
+        <v>0.8018795749997645</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179">
-        <v>0.000307098303788537</v>
+        <v>0.005143322799245328</v>
       </c>
       <c r="B179">
-        <v>0.9996929016962116</v>
+        <v>0.9948566772007545</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180">
-        <v>0.03494647715914782</v>
+        <v>0.1020606593919391</v>
       </c>
       <c r="B180">
-        <v>0.9650535228408522</v>
+        <v>0.8979393406080607</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181">
-        <v>0.0004070141166456246</v>
+        <v>0.005844613224015268</v>
       </c>
       <c r="B181">
-        <v>0.9995929858833544</v>
+        <v>0.9941553867759848</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182">
-        <v>1.566198341568607E-05</v>
+        <v>0.0007159794024611236</v>
       </c>
       <c r="B182">
-        <v>0.9999843380165844</v>
+        <v>0.9992840205975387</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183">
-        <v>0.03503587441137214</v>
+        <v>0.07682293413743914</v>
       </c>
       <c r="B183">
-        <v>0.9649641255886278</v>
+        <v>0.923177065862561</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184">
-        <v>0.001868500193297325</v>
+        <v>0.02530090689484695</v>
       </c>
       <c r="B184">
-        <v>0.9981314998067028</v>
+        <v>0.974699093105153</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185">
-        <v>0.6761929077181331</v>
+        <v>0.3855827602345083</v>
       </c>
       <c r="B185">
-        <v>0.3238070922818668</v>
+        <v>0.6144172397654917</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186">
-        <v>0.8903339956722172</v>
+        <v>0.865978223994128</v>
       </c>
       <c r="B186">
-        <v>0.1096660043277826</v>
+        <v>0.134021776005872</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187">
-        <v>0.9493935199662912</v>
+        <v>0.8025081524037689</v>
       </c>
       <c r="B187">
-        <v>0.05060648003370882</v>
+        <v>0.1974918475962311</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188">
-        <v>2.964680572466645E-05</v>
+        <v>0.0006951444195098928</v>
       </c>
       <c r="B188">
-        <v>0.9999703531942754</v>
+        <v>0.9993048555804903</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189">
-        <v>1.337255228524015E-05</v>
+        <v>0.0007256986106274195</v>
       </c>
       <c r="B189">
-        <v>0.9999866274477148</v>
+        <v>0.9992743013893726</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190">
-        <v>0.0003951862323886705</v>
+        <v>0.002206727218176141</v>
       </c>
       <c r="B190">
-        <v>0.9996048137676112</v>
+        <v>0.9977932727818238</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191">
-        <v>0.09228071914629797</v>
+        <v>0.1614108645600766</v>
       </c>
       <c r="B191">
-        <v>0.9077192808537018</v>
+        <v>0.8385891354399233</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192">
-        <v>0.7986461980832958</v>
+        <v>0.6983555732089353</v>
       </c>
       <c r="B192">
-        <v>0.2013538019167042</v>
+        <v>0.3016444267910646</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193">
-        <v>0.9391405693092366</v>
+        <v>0.587791588893381</v>
       </c>
       <c r="B193">
-        <v>0.06085943069076342</v>
+        <v>0.412208411106619</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194">
-        <v>0.007784007479677794</v>
+        <v>0.1639323397512284</v>
       </c>
       <c r="B194">
-        <v>0.9922159925203222</v>
+        <v>0.8360676602487715</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195">
-        <v>0.02585824838957294</v>
+        <v>0.02999856674150664</v>
       </c>
       <c r="B195">
-        <v>0.974141751610427</v>
+        <v>0.9700014332584934</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196">
-        <v>0.06859165588128482</v>
+        <v>0.02988291910763108</v>
       </c>
       <c r="B196">
-        <v>0.9314083441187151</v>
+        <v>0.9701170808923689</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197">
-        <v>0.01583765669861618</v>
+        <v>0.07437895804234428</v>
       </c>
       <c r="B197">
-        <v>0.9841623433013837</v>
+        <v>0.9256210419576558</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198">
-        <v>0.9162082831419283</v>
+        <v>0.7924479904943224</v>
       </c>
       <c r="B198">
-        <v>0.0837917168580716</v>
+        <v>0.2075520095056776</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199">
-        <v>0.03724617029725035</v>
+        <v>0.05879737181749186</v>
       </c>
       <c r="B199">
-        <v>0.9627538297027497</v>
+        <v>0.941202628182508</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200">
-        <v>1.56939411147361E-05</v>
+        <v>0.00128795530507051</v>
       </c>
       <c r="B200">
-        <v>0.9999843060588852</v>
+        <v>0.9987120446949295</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201">
-        <v>0.7027556664141902</v>
+        <v>0.5310101019015702</v>
       </c>
       <c r="B201">
-        <v>0.2972443335858098</v>
+        <v>0.4689898980984298</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202">
-        <v>3.452571609992757E-05</v>
+        <v>0.001204378723792924</v>
       </c>
       <c r="B202">
-        <v>0.9999654742839</v>
+        <v>0.998795621276207</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203">
-        <v>0.7763167973076975</v>
+        <v>0.547567306808503</v>
       </c>
       <c r="B203">
-        <v>0.2236832026923024</v>
+        <v>0.4524326931914971</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204">
-        <v>0.001492330595683759</v>
+        <v>0.03186972703774048</v>
       </c>
       <c r="B204">
-        <v>0.9985076694043163</v>
+        <v>0.9681302729622596</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205">
-        <v>0.01051255993935832</v>
+        <v>0.04448265378472557</v>
       </c>
       <c r="B205">
-        <v>0.9894874400606416</v>
+        <v>0.9555173462152745</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206">
-        <v>0.00191015607201069</v>
+        <v>0.004103261493127616</v>
       </c>
       <c r="B206">
-        <v>0.9980898439279893</v>
+        <v>0.9958967385068722</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207">
-        <v>0.8560532838789764</v>
+        <v>0.5677163018117927</v>
       </c>
       <c r="B207">
-        <v>0.1439467161210235</v>
+        <v>0.4322836981882074</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208">
-        <v>0.6174077609601233</v>
+        <v>0.2319591051325871</v>
       </c>
       <c r="B208">
-        <v>0.3825922390398768</v>
+        <v>0.768040894867413</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209">
-        <v>0.008855893585554823</v>
+        <v>0.03310664457957827</v>
       </c>
       <c r="B209">
-        <v>0.9911441064144453</v>
+        <v>0.9668933554204217</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210">
-        <v>0.8214233813731071</v>
+        <v>0.7849143545690239</v>
       </c>
       <c r="B210">
-        <v>0.1785766186268928</v>
+        <v>0.215085645430976</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211">
-        <v>0.02333359429855282</v>
+        <v>0.03546088423326969</v>
       </c>
       <c r="B211">
-        <v>0.9766664057014471</v>
+        <v>0.9645391157667303</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212">
-        <v>0.5672513099249057</v>
+        <v>0.3781268142256137</v>
       </c>
       <c r="B212">
-        <v>0.4327486900750943</v>
+        <v>0.6218731857743863</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213">
-        <v>0.001002175435331787</v>
+        <v>0.006759644438415628</v>
       </c>
       <c r="B213">
-        <v>0.9989978245646681</v>
+        <v>0.9932403555615844</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214">
-        <v>0.4477076618993821</v>
+        <v>0.2637246128352573</v>
       </c>
       <c r="B214">
-        <v>0.5522923381006178</v>
+        <v>0.7362753871647425</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215">
-        <v>0.0431375309860222</v>
+        <v>0.05716591636885517</v>
       </c>
       <c r="B215">
-        <v>0.9568624690139778</v>
+        <v>0.9428340836311448</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216">
-        <v>0.9151423331545452</v>
+        <v>0.6265006461855501</v>
       </c>
       <c r="B216">
-        <v>0.08485766684545466</v>
+        <v>0.3734993538144499</v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217">
-        <v>0.04883250372781047</v>
+        <v>0.04483813388574306</v>
       </c>
       <c r="B217">
-        <v>0.9511674962721897</v>
+        <v>0.9551618661142569</v>
       </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218">
-        <v>0.872265267844044</v>
+        <v>0.7170616902161489</v>
       </c>
       <c r="B218">
-        <v>0.127734732155956</v>
+        <v>0.2829383097838512</v>
       </c>
     </row>
     <row r="219" spans="1:2">
       <c r="A219">
-        <v>0.577225527024315</v>
+        <v>0.2553019378824931</v>
       </c>
       <c r="B219">
-        <v>0.4227744729756849</v>
+        <v>0.7446980621175069</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220">
-        <v>0.737176123896775</v>
+        <v>0.4186789825774661</v>
       </c>
       <c r="B220">
-        <v>0.262823876103225</v>
+        <v>0.5813210174225339</v>
       </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221">
-        <v>0.9697510824193628</v>
+        <v>0.9361899068855877</v>
       </c>
       <c r="B221">
-        <v>0.03024891758063722</v>
+        <v>0.0638100931144123</v>
       </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222">
-        <v>0.8940793150894993</v>
+        <v>0.6303320327131828</v>
       </c>
       <c r="B222">
-        <v>0.1059206849105006</v>
+        <v>0.3696679672868173</v>
       </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223">
-        <v>0.03949893899768862</v>
+        <v>0.114358218962745</v>
       </c>
       <c r="B223">
-        <v>0.9605010610023114</v>
+        <v>0.8856417810372552</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224">
-        <v>0.9727770980523823</v>
+        <v>0.7460113152061186</v>
       </c>
       <c r="B224">
-        <v>0.02722290194761784</v>
+        <v>0.2539886847938813</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225">
-        <v>0.4705640834959682</v>
+        <v>0.2985843124687985</v>
       </c>
       <c r="B225">
-        <v>0.5294359165040318</v>
+        <v>0.7014156875312014</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226">
-        <v>0.001463172601614748</v>
+        <v>0.004528585433049044</v>
       </c>
       <c r="B226">
-        <v>0.9985368273983852</v>
+        <v>0.9954714145669509</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227">
-        <v>0.08138926205164322</v>
+        <v>0.1022025203038001</v>
       </c>
       <c r="B227">
-        <v>0.918610737948357</v>
+        <v>0.8977974796961998</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228">
-        <v>0.4113198009139792</v>
+        <v>0.2559287295659594</v>
       </c>
       <c r="B228">
-        <v>0.5886801990860207</v>
+        <v>0.7440712704340405</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229">
-        <v>0.04435699011934307</v>
+        <v>0.053119579665535</v>
       </c>
       <c r="B229">
-        <v>0.9556430098806568</v>
+        <v>0.946880420334465</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230">
-        <v>0.9464016760914034</v>
+        <v>0.7533854276692715</v>
       </c>
       <c r="B230">
-        <v>0.05359832390859674</v>
+        <v>0.2466145723307285</v>
       </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231">
-        <v>0.5392044497861951</v>
+        <v>0.3548293578798778</v>
       </c>
       <c r="B231">
-        <v>0.4607955502138049</v>
+        <v>0.6451706421201222</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232">
-        <v>0.5637957358828646</v>
+        <v>0.3077035675699333</v>
       </c>
       <c r="B232">
-        <v>0.4362042641171355</v>
+        <v>0.6922964324300668</v>
       </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233">
-        <v>8.892829052036255E-05</v>
+        <v>0.0006635366942324102</v>
       </c>
       <c r="B233">
-        <v>0.9999110717094797</v>
+        <v>0.9993364633057674</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234">
-        <v>0.883491419065113</v>
+        <v>0.6565859776670032</v>
       </c>
       <c r="B234">
-        <v>0.116508580934887</v>
+        <v>0.3434140223329969</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Local training loss : .23 , validation loss : .27, online loss : 0.33671 rank : 102, 20:48pm
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -382,1866 +382,1866 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>0.002590812557503027</v>
+        <v>1.802217817903065E-08</v>
       </c>
       <c r="B2">
-        <v>0.997409187442497</v>
+        <v>0.9999999819778218</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>0.2961098999981138</v>
+        <v>0.02233717110904001</v>
       </c>
       <c r="B3">
-        <v>0.7038901000018861</v>
+        <v>0.97766282889096</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>0.663527563210501</v>
+        <v>0.8359954899863614</v>
       </c>
       <c r="B4">
-        <v>0.336472436789499</v>
+        <v>0.1640045100136386</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>0.00476154464118325</v>
+        <v>8.172819682634237E-08</v>
       </c>
       <c r="B5">
-        <v>0.9952384553588166</v>
+        <v>0.9999999182718031</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>0.398451998699122</v>
+        <v>0.7482392758342933</v>
       </c>
       <c r="B6">
-        <v>0.601548001300878</v>
+        <v>0.2517607241657067</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>0.6460110409111197</v>
+        <v>0.8097772996028794</v>
       </c>
       <c r="B7">
-        <v>0.3539889590888801</v>
+        <v>0.1902227003971206</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>0.742508921247145</v>
+        <v>0.8089018556960788</v>
       </c>
       <c r="B8">
-        <v>0.2574910787528552</v>
+        <v>0.1910981443039213</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>0.850922884269649</v>
+        <v>0.8270888296414367</v>
       </c>
       <c r="B9">
-        <v>0.1490771157303509</v>
+        <v>0.1729111703585634</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>0.02360250528078069</v>
+        <v>0.007803935721371238</v>
       </c>
       <c r="B10">
-        <v>0.9763974947192192</v>
+        <v>0.9921960642786288</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>0.01220786208729949</v>
+        <v>3.380614812398565E-07</v>
       </c>
       <c r="B11">
-        <v>0.9877921379127006</v>
+        <v>0.9999996619385186</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>0.04321889005179715</v>
+        <v>0.01139706381235498</v>
       </c>
       <c r="B12">
-        <v>0.9567811099482029</v>
+        <v>0.9886029361876451</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>0.8588827350961352</v>
+        <v>0.8191439963625572</v>
       </c>
       <c r="B13">
-        <v>0.1411172649038649</v>
+        <v>0.1808560036374429</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>0.4488096279818531</v>
+        <v>0.7088776717264377</v>
       </c>
       <c r="B14">
-        <v>0.5511903720181468</v>
+        <v>0.2911223282735624</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>0.5381287818690833</v>
+        <v>0.8143798348899537</v>
       </c>
       <c r="B15">
-        <v>0.4618712181309167</v>
+        <v>0.1856201651100464</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>0.0141637610495182</v>
+        <v>5.935700107600936E-07</v>
       </c>
       <c r="B16">
-        <v>0.9858362389504817</v>
+        <v>0.9999994064299894</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>0.8221532667474605</v>
+        <v>0.803549240466167</v>
       </c>
       <c r="B17">
-        <v>0.1778467332525395</v>
+        <v>0.196450759533833</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>0.514903875079726</v>
+        <v>0.771399514952456</v>
       </c>
       <c r="B18">
-        <v>0.485096124920274</v>
+        <v>0.228600485047544</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>0.4126876791528929</v>
+        <v>0.7650469829813353</v>
       </c>
       <c r="B19">
-        <v>0.5873123208471072</v>
+        <v>0.2349530170186646</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>0.06464216865605026</v>
+        <v>0.02722440540223804</v>
       </c>
       <c r="B20">
-        <v>0.9353578313439498</v>
+        <v>0.972775594597762</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>0.001701629327904904</v>
+        <v>1.350927823752162E-08</v>
       </c>
       <c r="B21">
-        <v>0.9982983706720951</v>
+        <v>0.9999999864907216</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>0.6331309524642089</v>
+        <v>0.7398826836719994</v>
       </c>
       <c r="B22">
-        <v>0.366869047535791</v>
+        <v>0.2601173163280008</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>0.3713127900190087</v>
+        <v>0.7852328744320105</v>
       </c>
       <c r="B23">
-        <v>0.6286872099809914</v>
+        <v>0.2147671255679893</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>0.3309419741519523</v>
+        <v>0.02816075195574778</v>
       </c>
       <c r="B24">
-        <v>0.6690580258480476</v>
+        <v>0.9718392480442521</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>0.9232090623978889</v>
+        <v>0.8141517680931685</v>
       </c>
       <c r="B25">
-        <v>0.07679093760211116</v>
+        <v>0.1858482319068316</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>0.7323956862780158</v>
+        <v>0.8157500386011491</v>
       </c>
       <c r="B26">
-        <v>0.2676043137219845</v>
+        <v>0.1842499613988509</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>0.008458869919169547</v>
+        <v>1.582315068506181E-06</v>
       </c>
       <c r="B27">
-        <v>0.9915411300808302</v>
+        <v>0.9999984176849316</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>0.4690468282515542</v>
+        <v>0.7578412750643658</v>
       </c>
       <c r="B28">
-        <v>0.5309531717484458</v>
+        <v>0.2421587249356341</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>0.0007412209456209018</v>
+        <v>6.645015655229333E-09</v>
       </c>
       <c r="B29">
-        <v>0.999258779054379</v>
+        <v>0.9999999933549845</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>0.02131428114060944</v>
+        <v>3.245799057343648E-07</v>
       </c>
       <c r="B30">
-        <v>0.9786857188593905</v>
+        <v>0.9999996754200943</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>0.8855794020913983</v>
+        <v>0.7633293449021437</v>
       </c>
       <c r="B31">
-        <v>0.1144205979086017</v>
+        <v>0.2366706550978562</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>0.6920290719051596</v>
+        <v>0.7450822903872091</v>
       </c>
       <c r="B32">
-        <v>0.3079709280948403</v>
+        <v>0.2549177096127909</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>0.01934906934302971</v>
+        <v>0.001827960809700097</v>
       </c>
       <c r="B33">
-        <v>0.9806509306569704</v>
+        <v>0.9981720391902997</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
-        <v>0.04868653033919248</v>
+        <v>0.01234204705198313</v>
       </c>
       <c r="B34">
-        <v>0.9513134696608074</v>
+        <v>0.9876579529480168</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>0.001066210096426201</v>
+        <v>8.136131081225287E-08</v>
       </c>
       <c r="B35">
-        <v>0.9989337899035738</v>
+        <v>0.9999999186386891</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>0.6832424629037621</v>
+        <v>0.785314909837261</v>
       </c>
       <c r="B36">
-        <v>0.3167575370962379</v>
+        <v>0.2146850901627391</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>0.8543998471527856</v>
+        <v>0.8114022183676746</v>
       </c>
       <c r="B37">
-        <v>0.1456001528472144</v>
+        <v>0.1885977816323256</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38">
-        <v>0.00103063586318423</v>
+        <v>6.16721803865173E-09</v>
       </c>
       <c r="B38">
-        <v>0.9989693641368158</v>
+        <v>0.9999999938327818</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39">
-        <v>0.7767970250585622</v>
+        <v>0.8344472409517464</v>
       </c>
       <c r="B39">
-        <v>0.2232029749414378</v>
+        <v>0.1655527590482537</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40">
-        <v>0.8275280027291133</v>
+        <v>0.8349063419431929</v>
       </c>
       <c r="B40">
-        <v>0.1724719972708866</v>
+        <v>0.1650936580568071</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41">
-        <v>0.7909627768694917</v>
+        <v>0.830714929816477</v>
       </c>
       <c r="B41">
-        <v>0.2090372231305084</v>
+        <v>0.169285070183523</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42">
-        <v>0.02636708730558874</v>
+        <v>0.0003132558994790561</v>
       </c>
       <c r="B42">
-        <v>0.9736329126944113</v>
+        <v>0.9996867441005211</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43">
-        <v>0.6927212729613571</v>
+        <v>0.798866248168709</v>
       </c>
       <c r="B43">
-        <v>0.3072787270386428</v>
+        <v>0.2011337518312909</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44">
-        <v>0.43531087566325</v>
+        <v>0.7668831819829877</v>
       </c>
       <c r="B44">
-        <v>0.56468912433675</v>
+        <v>0.2331168180170123</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45">
-        <v>0.6288924232004437</v>
+        <v>0.8099386947426541</v>
       </c>
       <c r="B45">
-        <v>0.3711075767995562</v>
+        <v>0.1900613052573459</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46">
-        <v>0.001959313437407776</v>
+        <v>1.072743482108522E-08</v>
       </c>
       <c r="B46">
-        <v>0.9980406865625923</v>
+        <v>0.9999999892725652</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47">
-        <v>0.5597428669104654</v>
+        <v>0.7161532056364184</v>
       </c>
       <c r="B47">
-        <v>0.4402571330895346</v>
+        <v>0.2838467943635816</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48">
-        <v>0.6252277911431012</v>
+        <v>0.8227660945448261</v>
       </c>
       <c r="B48">
-        <v>0.3747722088568988</v>
+        <v>0.1772339054551739</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49">
-        <v>0.0006229617456471548</v>
+        <v>8.551658332543108E-09</v>
       </c>
       <c r="B49">
-        <v>0.9993770382543529</v>
+        <v>0.9999999914483415</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50">
-        <v>0.04851474348036501</v>
+        <v>0.01617635010182434</v>
       </c>
       <c r="B50">
-        <v>0.9514852565196349</v>
+        <v>0.9838236498981755</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51">
-        <v>0.2785993415916615</v>
+        <v>0.02900221931126824</v>
       </c>
       <c r="B51">
-        <v>0.7214006584083384</v>
+        <v>0.9709977806887317</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52">
-        <v>0.3016010153704168</v>
+        <v>0.02809359223262017</v>
       </c>
       <c r="B52">
-        <v>0.6983989846295832</v>
+        <v>0.9719064077673797</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53">
-        <v>0.03387900147435963</v>
+        <v>0.01519909839506124</v>
       </c>
       <c r="B53">
-        <v>0.9661209985256404</v>
+        <v>0.9848009016049389</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54">
-        <v>0.7876639588813312</v>
+        <v>0.8502819959749049</v>
       </c>
       <c r="B54">
-        <v>0.2123360411186688</v>
+        <v>0.1497180040250953</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55">
-        <v>0.04378216898041284</v>
+        <v>8.334804742373615E-07</v>
       </c>
       <c r="B55">
-        <v>0.9562178310195873</v>
+        <v>0.9999991665195259</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56">
-        <v>0.2552023908413459</v>
+        <v>0.7508941466138239</v>
       </c>
       <c r="B56">
-        <v>0.7447976091586541</v>
+        <v>0.2491058533861759</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57">
-        <v>0.468719310983933</v>
+        <v>0.8050042415722864</v>
       </c>
       <c r="B57">
-        <v>0.5312806890160668</v>
+        <v>0.1949957584277136</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58">
-        <v>0.00205905836998818</v>
+        <v>9.076687264039568E-08</v>
       </c>
       <c r="B58">
-        <v>0.9979409416300119</v>
+        <v>0.9999999092331273</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59">
-        <v>0.7136785574887627</v>
+        <v>0.709174748525994</v>
       </c>
       <c r="B59">
-        <v>0.2863214425112372</v>
+        <v>0.290825251474006</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60">
-        <v>0.7117334786189282</v>
+        <v>0.8297287729042718</v>
       </c>
       <c r="B60">
-        <v>0.2882665213810718</v>
+        <v>0.1702712270957282</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61">
-        <v>0.1729095535964272</v>
+        <v>0.7317994381332443</v>
       </c>
       <c r="B61">
-        <v>0.8270904464035727</v>
+        <v>0.2682005618667558</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62">
-        <v>0.878020559129716</v>
+        <v>0.8061958495777296</v>
       </c>
       <c r="B62">
-        <v>0.121979440870284</v>
+        <v>0.1938041504222706</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63">
-        <v>0.7603611691566112</v>
+        <v>0.8382930007389201</v>
       </c>
       <c r="B63">
-        <v>0.2396388308433887</v>
+        <v>0.16170699926108</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64">
-        <v>0.1403998638822483</v>
+        <v>0.7036560260964609</v>
       </c>
       <c r="B64">
-        <v>0.8596001361177517</v>
+        <v>0.2963439739035391</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65">
-        <v>0.2235826217871664</v>
+        <v>0.0182813695167148</v>
       </c>
       <c r="B65">
-        <v>0.7764173782128335</v>
+        <v>0.9817186304832852</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66">
-        <v>0.5519814470004765</v>
+        <v>0.7563055306525768</v>
       </c>
       <c r="B66">
-        <v>0.4480185529995235</v>
+        <v>0.2436944693474233</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67">
-        <v>0.5437010513940181</v>
+        <v>0.8080428255270714</v>
       </c>
       <c r="B67">
-        <v>0.4562989486059819</v>
+        <v>0.1919571744729285</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68">
-        <v>0.009124588552720655</v>
+        <v>1.669053346241361E-07</v>
       </c>
       <c r="B68">
-        <v>0.9908754114472792</v>
+        <v>0.9999998330946656</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69">
-        <v>0.7899445828938207</v>
+        <v>0.7669849533538403</v>
       </c>
       <c r="B69">
-        <v>0.2100554171061792</v>
+        <v>0.2330150466461595</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70">
-        <v>0.2362239917412662</v>
+        <v>0.7672406321715464</v>
       </c>
       <c r="B70">
-        <v>0.7637760082587339</v>
+        <v>0.2327593678284537</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71">
-        <v>0.6463657618386142</v>
+        <v>0.8072070463592155</v>
       </c>
       <c r="B71">
-        <v>0.3536342381613859</v>
+        <v>0.1927929536407844</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72">
-        <v>0.5808074426767711</v>
+        <v>0.7676860929284085</v>
       </c>
       <c r="B72">
-        <v>0.419192557323229</v>
+        <v>0.2323139070715914</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73">
-        <v>0.0009024998518503505</v>
+        <v>1.125817153266947E-08</v>
       </c>
       <c r="B73">
-        <v>0.9990975001481496</v>
+        <v>0.9999999887418284</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74">
-        <v>0.009959005844862801</v>
+        <v>2.961820217441106E-07</v>
       </c>
       <c r="B74">
-        <v>0.9900409941551371</v>
+        <v>0.9999997038179784</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75">
-        <v>0.0008863199936380999</v>
+        <v>6.315554269086327E-08</v>
       </c>
       <c r="B75">
-        <v>0.9991136800063618</v>
+        <v>0.9999999368444571</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76">
-        <v>0.3212612993806395</v>
+        <v>0.6881374969379821</v>
       </c>
       <c r="B76">
-        <v>0.6787387006193605</v>
+        <v>0.3118625030620178</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77">
-        <v>0.009508694925771369</v>
+        <v>1.613704265788119E-06</v>
       </c>
       <c r="B77">
-        <v>0.9904913050742288</v>
+        <v>0.9999983862957342</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78">
-        <v>0.4738531767303711</v>
+        <v>0.7578446489231758</v>
       </c>
       <c r="B78">
-        <v>0.5261468232696287</v>
+        <v>0.2421553510768241</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79">
-        <v>0.003808310730531613</v>
+        <v>3.721429884153516E-07</v>
       </c>
       <c r="B79">
-        <v>0.9961916892694682</v>
+        <v>0.9999996278570116</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80">
-        <v>0.5659603917004732</v>
+        <v>0.7898927208441566</v>
       </c>
       <c r="B80">
-        <v>0.4340396082995268</v>
+        <v>0.2101072791558433</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81">
-        <v>0.009810007470646398</v>
+        <v>5.002494051896404E-07</v>
       </c>
       <c r="B81">
-        <v>0.9901899925293536</v>
+        <v>0.9999994997505948</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82">
-        <v>0.0006759827005721124</v>
+        <v>8.309280854237409E-09</v>
       </c>
       <c r="B82">
-        <v>0.9993240172994278</v>
+        <v>0.9999999916907192</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83">
-        <v>0.2377673209753183</v>
+        <v>0.02764119639291328</v>
       </c>
       <c r="B83">
-        <v>0.7622326790246817</v>
+        <v>0.9723588036070868</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84">
-        <v>0.4267467998462292</v>
+        <v>0.7631579217248755</v>
       </c>
       <c r="B84">
-        <v>0.5732532001537708</v>
+        <v>0.2368420782751245</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85">
-        <v>0.774845233113815</v>
+        <v>0.7835222203756977</v>
       </c>
       <c r="B85">
-        <v>0.225154766886185</v>
+        <v>0.2164777796243023</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86">
-        <v>0.7671014288503615</v>
+        <v>0.8487633810910959</v>
       </c>
       <c r="B86">
-        <v>0.2328985711496384</v>
+        <v>0.1512366189089039</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87">
-        <v>0.9249464821194667</v>
+        <v>0.8143957640124602</v>
       </c>
       <c r="B87">
-        <v>0.07505351788053324</v>
+        <v>0.1856042359875399</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88">
-        <v>0.002022329040128904</v>
+        <v>1.340557476894995E-08</v>
       </c>
       <c r="B88">
-        <v>0.9979776709598712</v>
+        <v>0.9999999865944253</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89">
-        <v>0.1945814419381248</v>
+        <v>0.6982999807779954</v>
       </c>
       <c r="B89">
-        <v>0.8054185580618752</v>
+        <v>0.3017000192220046</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90">
-        <v>0.6687589415762829</v>
+        <v>0.7546099102244284</v>
       </c>
       <c r="B90">
-        <v>0.331241058423717</v>
+        <v>0.2453900897755715</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91">
-        <v>0.7665442300570452</v>
+        <v>0.05354917283028261</v>
       </c>
       <c r="B91">
-        <v>0.2334557699429547</v>
+        <v>0.9464508271697174</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92">
-        <v>0.5085328407418132</v>
+        <v>0.7958736957393523</v>
       </c>
       <c r="B92">
-        <v>0.4914671592581869</v>
+        <v>0.2041263042606477</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93">
-        <v>0.083625515075608</v>
+        <v>0.01260557221566753</v>
       </c>
       <c r="B93">
-        <v>0.9163744849243918</v>
+        <v>0.9873944277843325</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94">
-        <v>0.07871527502264462</v>
+        <v>0.01672427724675871</v>
       </c>
       <c r="B94">
-        <v>0.9212847249773556</v>
+        <v>0.9832757227532412</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95">
-        <v>0.7765516832600661</v>
+        <v>0.8199753267070737</v>
       </c>
       <c r="B95">
-        <v>0.2234483167399342</v>
+        <v>0.1800246732929262</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96">
-        <v>0.005109621441824215</v>
+        <v>4.733326720340714E-07</v>
       </c>
       <c r="B96">
-        <v>0.9948903785581759</v>
+        <v>0.9999995266673277</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97">
-        <v>0.006071504926609002</v>
+        <v>1.255159604416307E-07</v>
       </c>
       <c r="B97">
-        <v>0.9939284950733911</v>
+        <v>0.9999998744840396</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98">
-        <v>0.5965394025157755</v>
+        <v>0.781347611051658</v>
       </c>
       <c r="B98">
-        <v>0.4034605974842245</v>
+        <v>0.2186523889483421</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99">
-        <v>0.5295407910576</v>
+        <v>0.837090104544676</v>
       </c>
       <c r="B99">
-        <v>0.4704592089424001</v>
+        <v>0.162909895455324</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100">
-        <v>0.5886327975928914</v>
+        <v>0.7877921924961639</v>
       </c>
       <c r="B100">
-        <v>0.4113672024071085</v>
+        <v>0.2122078075038362</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101">
-        <v>0.03252347816527927</v>
+        <v>0.01423162998243124</v>
       </c>
       <c r="B101">
-        <v>0.9674765218347205</v>
+        <v>0.9857683700175688</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102">
-        <v>0.4355087253500961</v>
+        <v>0.8049428542233792</v>
       </c>
       <c r="B102">
-        <v>0.5644912746499038</v>
+        <v>0.1950571457766207</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103">
-        <v>0.8109942870042665</v>
+        <v>0.857983900937408</v>
       </c>
       <c r="B103">
-        <v>0.1890057129957336</v>
+        <v>0.1420160990625921</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104">
-        <v>0.001514267255451814</v>
+        <v>1.726251182283477E-08</v>
       </c>
       <c r="B104">
-        <v>0.998485732744548</v>
+        <v>0.9999999827374881</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105">
-        <v>0.3076808199273238</v>
+        <v>0.0289652056682883</v>
       </c>
       <c r="B105">
-        <v>0.6923191800726763</v>
+        <v>0.9710347943317118</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106">
-        <v>0.5749832951361574</v>
+        <v>0.810462807668944</v>
       </c>
       <c r="B106">
-        <v>0.4250167048638425</v>
+        <v>0.189537192331056</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107">
-        <v>0.000588262384925442</v>
+        <v>1.284786488909663E-08</v>
       </c>
       <c r="B107">
-        <v>0.9994117376150746</v>
+        <v>0.9999999871521351</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108">
-        <v>0.5669722126966978</v>
+        <v>0.8172356025623714</v>
       </c>
       <c r="B108">
-        <v>0.4330277873033021</v>
+        <v>0.1827643974376287</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109">
-        <v>0.001119737329347581</v>
+        <v>3.683149137902511E-08</v>
       </c>
       <c r="B109">
-        <v>0.9988802626706524</v>
+        <v>0.9999999631685086</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110">
-        <v>0.4092669766575656</v>
+        <v>0.8111095325407871</v>
       </c>
       <c r="B110">
-        <v>0.5907330233424344</v>
+        <v>0.1888904674592128</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111">
-        <v>0.001228832615315115</v>
+        <v>1.80726005753337E-08</v>
       </c>
       <c r="B111">
-        <v>0.998771167384685</v>
+        <v>0.9999999819273995</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112">
-        <v>0.7759297157467985</v>
+        <v>0.776477550780572</v>
       </c>
       <c r="B112">
-        <v>0.2240702842532015</v>
+        <v>0.223522449219428</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113">
-        <v>0.4744786019015698</v>
+        <v>0.7900473264664748</v>
       </c>
       <c r="B113">
-        <v>0.52552139809843</v>
+        <v>0.2099526735335253</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114">
-        <v>0.03400757453859102</v>
+        <v>0.01489706175624889</v>
       </c>
       <c r="B114">
-        <v>0.965992425461409</v>
+        <v>0.9851029382437509</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115">
-        <v>0.6907844907695541</v>
+        <v>0.7945244125946836</v>
       </c>
       <c r="B115">
-        <v>0.3092155092304461</v>
+        <v>0.2054755874053163</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116">
-        <v>0.5799032957125896</v>
+        <v>0.7828770340473151</v>
       </c>
       <c r="B116">
-        <v>0.4200967042874106</v>
+        <v>0.2171229659526848</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117">
-        <v>0.1425547565239791</v>
+        <v>0.02314538760968599</v>
       </c>
       <c r="B117">
-        <v>0.8574452434760208</v>
+        <v>0.976854612390314</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118">
-        <v>0.0006963264615153619</v>
+        <v>1.0547697775961E-08</v>
       </c>
       <c r="B118">
-        <v>0.9993036735384848</v>
+        <v>0.9999999894523021</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119">
-        <v>0.1572712088348775</v>
+        <v>0.01771403898345384</v>
       </c>
       <c r="B119">
-        <v>0.8427287911651226</v>
+        <v>0.982285961016546</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120">
-        <v>0.03479643780649599</v>
+        <v>1.2262832207755E-06</v>
       </c>
       <c r="B120">
-        <v>0.9652035621935039</v>
+        <v>0.9999987737167793</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121">
-        <v>0.001203812000249919</v>
+        <v>1.261912725800611E-08</v>
       </c>
       <c r="B121">
-        <v>0.9987961879997499</v>
+        <v>0.9999999873808728</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122">
-        <v>0.4530384306837048</v>
+        <v>0.775764960790875</v>
       </c>
       <c r="B122">
-        <v>0.5469615693162952</v>
+        <v>0.224235039209125</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123">
-        <v>0.004751896368102493</v>
+        <v>1.771089457238462E-07</v>
       </c>
       <c r="B123">
-        <v>0.9952481036318975</v>
+        <v>0.9999998228910543</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124">
-        <v>0.8798493411556078</v>
+        <v>0.8178090169646768</v>
       </c>
       <c r="B124">
-        <v>0.1201506588443922</v>
+        <v>0.1821909830353232</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125">
-        <v>0.8095122277133461</v>
+        <v>0.8165273653402203</v>
       </c>
       <c r="B125">
-        <v>0.1904877722866539</v>
+        <v>0.1834726346597798</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126">
-        <v>0.6341574993664624</v>
+        <v>0.8399686655509552</v>
       </c>
       <c r="B126">
-        <v>0.3658425006335377</v>
+        <v>0.1600313344490448</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127">
-        <v>0.0006561318421529776</v>
+        <v>1.266751386881255E-08</v>
       </c>
       <c r="B127">
-        <v>0.9993438681578469</v>
+        <v>0.9999999873324863</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128">
-        <v>0.3469900355961011</v>
+        <v>0.8105671446365084</v>
       </c>
       <c r="B128">
-        <v>0.6530099644038987</v>
+        <v>0.1894328553634915</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129">
-        <v>0.08889688959209328</v>
+        <v>0.01399194701421732</v>
       </c>
       <c r="B129">
-        <v>0.9111031104079067</v>
+        <v>0.9860080529857825</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130">
-        <v>0.1948099081734133</v>
+        <v>0.0212381407982483</v>
       </c>
       <c r="B130">
-        <v>0.8051900918265866</v>
+        <v>0.9787618592017518</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131">
-        <v>0.03738446629762401</v>
+        <v>0.01438965554347544</v>
       </c>
       <c r="B131">
-        <v>0.9626155337023762</v>
+        <v>0.9856103444565245</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132">
-        <v>0.7904158233534154</v>
+        <v>0.8119032889051684</v>
       </c>
       <c r="B132">
-        <v>0.2095841766465846</v>
+        <v>0.1880967110948317</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133">
-        <v>0.7613240637978694</v>
+        <v>0.8506461593624338</v>
       </c>
       <c r="B133">
-        <v>0.2386759362021307</v>
+        <v>0.149353840637566</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134">
-        <v>0.9611047494386956</v>
+        <v>0.7602078180889091</v>
       </c>
       <c r="B134">
-        <v>0.03889525056130426</v>
+        <v>0.2397921819110908</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135">
-        <v>0.6213391731258903</v>
+        <v>0.8226245255984806</v>
       </c>
       <c r="B135">
-        <v>0.3786608268741097</v>
+        <v>0.1773754744015195</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136">
-        <v>0.004949604284314946</v>
+        <v>4.157748923330357E-07</v>
       </c>
       <c r="B136">
-        <v>0.995050395715685</v>
+        <v>0.9999995842251077</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137">
-        <v>0.03479812875665058</v>
+        <v>2.22801036551405E-06</v>
       </c>
       <c r="B137">
-        <v>0.9652018712433494</v>
+        <v>0.9999977719896347</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138">
-        <v>0.07509338137794448</v>
+        <v>0.01906817181706768</v>
       </c>
       <c r="B138">
-        <v>0.9249066186220556</v>
+        <v>0.9809318281829323</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139">
-        <v>0.4561876046703849</v>
+        <v>0.7764452833128364</v>
       </c>
       <c r="B139">
-        <v>0.543812395329615</v>
+        <v>0.2235547166871635</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140">
-        <v>0.7690596056496053</v>
+        <v>0.8061996401108701</v>
       </c>
       <c r="B140">
-        <v>0.2309403943503948</v>
+        <v>0.1938003598891299</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141">
-        <v>0.5481643633461737</v>
+        <v>0.751430527264926</v>
       </c>
       <c r="B141">
-        <v>0.4518356366538265</v>
+        <v>0.2485694727350741</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142">
-        <v>0.01368796923828695</v>
+        <v>1.431745383802271E-06</v>
       </c>
       <c r="B142">
-        <v>0.9863120307617129</v>
+        <v>0.9999985682546163</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143">
-        <v>0.4952416361450793</v>
+        <v>0.8330876957192259</v>
       </c>
       <c r="B143">
-        <v>0.5047583638549206</v>
+        <v>0.1669123042807742</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144">
-        <v>0.05700901028761648</v>
+        <v>0.01525292944987896</v>
       </c>
       <c r="B144">
-        <v>0.9429909897123836</v>
+        <v>0.984747070550121</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145">
-        <v>0.2840373887971593</v>
+        <v>0.01463231715464687</v>
       </c>
       <c r="B145">
-        <v>0.7159626112028407</v>
+        <v>0.9853676828453533</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146">
-        <v>0.6756353668572163</v>
+        <v>0.7740423832200275</v>
       </c>
       <c r="B146">
-        <v>0.3243646331427837</v>
+        <v>0.2259576167799726</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147">
-        <v>0.0704472043568337</v>
+        <v>0.02241548673308649</v>
       </c>
       <c r="B147">
-        <v>0.9295527956431663</v>
+        <v>0.9775845132669133</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148">
-        <v>0.0005456985886222565</v>
+        <v>1.173792837382365E-08</v>
       </c>
       <c r="B148">
-        <v>0.9994543014113775</v>
+        <v>0.9999999882620716</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149">
-        <v>0.002363181306236265</v>
+        <v>1.15970029605617E-08</v>
       </c>
       <c r="B149">
-        <v>0.9976368186937636</v>
+        <v>0.9999999884029971</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150">
-        <v>0.4659526000419862</v>
+        <v>0.7209815210322327</v>
       </c>
       <c r="B150">
-        <v>0.5340473999580139</v>
+        <v>0.2790184789677672</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151">
-        <v>0.5353172942096829</v>
+        <v>0.7894293133572934</v>
       </c>
       <c r="B151">
-        <v>0.4646827057903172</v>
+        <v>0.2105706866427066</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152">
-        <v>0.002995361565081075</v>
+        <v>2.827485400361242E-07</v>
       </c>
       <c r="B152">
-        <v>0.997004638434919</v>
+        <v>0.9999997172514601</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153">
-        <v>0.6135243246666252</v>
+        <v>0.7378045055308431</v>
       </c>
       <c r="B153">
-        <v>0.3864756753333748</v>
+        <v>0.2621954944691569</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154">
-        <v>0.3966946541837307</v>
+        <v>0.8320216602074932</v>
       </c>
       <c r="B154">
-        <v>0.6033053458162694</v>
+        <v>0.1679783397925066</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155">
-        <v>0.658161176928902</v>
+        <v>0.8542948225796526</v>
       </c>
       <c r="B155">
-        <v>0.341838823071098</v>
+        <v>0.1457051774203473</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156">
-        <v>0.4336142931049014</v>
+        <v>0.05094690938141268</v>
       </c>
       <c r="B156">
-        <v>0.5663857068950986</v>
+        <v>0.9490530906185873</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157">
-        <v>0.257522396451752</v>
+        <v>0.7062725755243524</v>
       </c>
       <c r="B157">
-        <v>0.7424776035482481</v>
+        <v>0.2937274244756475</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158">
-        <v>0.5060218492154073</v>
+        <v>0.7851452116357351</v>
       </c>
       <c r="B158">
-        <v>0.4939781507845928</v>
+        <v>0.2148547883642648</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159">
-        <v>0.003112229431723801</v>
+        <v>1.91422378424901E-07</v>
       </c>
       <c r="B159">
-        <v>0.9968877705682762</v>
+        <v>0.9999998085776215</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160">
-        <v>0.2336565535799202</v>
+        <v>0.02049598465563862</v>
       </c>
       <c r="B160">
-        <v>0.7663434464200799</v>
+        <v>0.9795040153443613</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161">
-        <v>0.004954213260234345</v>
+        <v>4.685638123232403E-08</v>
       </c>
       <c r="B161">
-        <v>0.9950457867397656</v>
+        <v>0.9999999531436188</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162">
-        <v>0.001034959681902466</v>
+        <v>5.363962922183583E-09</v>
       </c>
       <c r="B162">
-        <v>0.9989650403180976</v>
+        <v>0.9999999946360369</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163">
-        <v>0.6400848240299903</v>
+        <v>0.8235711449761912</v>
       </c>
       <c r="B163">
-        <v>0.3599151759700096</v>
+        <v>0.1764288550238089</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164">
-        <v>0.9096153970464155</v>
+        <v>0.8476172887353652</v>
       </c>
       <c r="B164">
-        <v>0.09038460295358459</v>
+        <v>0.1523827112646349</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165">
-        <v>0.2413494880935339</v>
+        <v>0.5790967546441408</v>
       </c>
       <c r="B165">
-        <v>0.7586505119064662</v>
+        <v>0.4209032453558592</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166">
-        <v>0.04914030473778152</v>
+        <v>0.01240613510603458</v>
       </c>
       <c r="B166">
-        <v>0.9508596952622186</v>
+        <v>0.9875938648939655</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167">
-        <v>0.4172344587377958</v>
+        <v>0.7846921479820018</v>
       </c>
       <c r="B167">
-        <v>0.582765541262204</v>
+        <v>0.2153078520179982</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168">
-        <v>0.3486599168647192</v>
+        <v>0.7396651531253199</v>
       </c>
       <c r="B168">
-        <v>0.6513400831352809</v>
+        <v>0.2603348468746799</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169">
-        <v>0.0494135615771493</v>
+        <v>0.004056315656069232</v>
       </c>
       <c r="B169">
-        <v>0.9505864384228506</v>
+        <v>0.9959436843439309</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170">
-        <v>0.001428448723904574</v>
+        <v>1.162675064292102E-08</v>
       </c>
       <c r="B170">
-        <v>0.9985715512760954</v>
+        <v>0.9999999883732493</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171">
-        <v>0.5263833587778897</v>
+        <v>0.8352417656913205</v>
       </c>
       <c r="B171">
-        <v>0.4736166412221103</v>
+        <v>0.1647582343086795</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172">
-        <v>0.0005991239487194821</v>
+        <v>1.306059430410846E-08</v>
       </c>
       <c r="B172">
-        <v>0.9994008760512804</v>
+        <v>0.9999999869394056</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173">
-        <v>0.03426089819071576</v>
+        <v>2.758097125203428E-07</v>
       </c>
       <c r="B173">
-        <v>0.9657391018092842</v>
+        <v>0.9999997241902873</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174">
-        <v>0.001334411591162328</v>
+        <v>1.954779568937117E-08</v>
       </c>
       <c r="B174">
-        <v>0.9986655884088377</v>
+        <v>0.9999999804522044</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175">
-        <v>0.6920377743422874</v>
+        <v>0.8106356932890049</v>
       </c>
       <c r="B175">
-        <v>0.3079622256577126</v>
+        <v>0.1893643067109951</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176">
-        <v>0.7316990341238169</v>
+        <v>0.7749794789943363</v>
       </c>
       <c r="B176">
-        <v>0.268300965876183</v>
+        <v>0.2250205210056637</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177">
-        <v>0.04629917033905275</v>
+        <v>0.01515546353264757</v>
       </c>
       <c r="B177">
-        <v>0.9537008296609473</v>
+        <v>0.9848445364673524</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178">
-        <v>0.1981204250002354</v>
+        <v>0.6653900063619079</v>
       </c>
       <c r="B178">
-        <v>0.8018795749997645</v>
+        <v>0.334609993638092</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179">
-        <v>0.005143322799245328</v>
+        <v>1.169785256160223E-06</v>
       </c>
       <c r="B179">
-        <v>0.9948566772007545</v>
+        <v>0.9999988302147439</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180">
-        <v>0.1020606593919391</v>
+        <v>0.02504690974800098</v>
       </c>
       <c r="B180">
-        <v>0.8979393406080607</v>
+        <v>0.9749530902519989</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181">
-        <v>0.005844613224015268</v>
+        <v>1.946696998974893E-07</v>
       </c>
       <c r="B181">
-        <v>0.9941553867759848</v>
+        <v>0.9999998053303</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182">
-        <v>0.0007159794024611236</v>
+        <v>1.99824826070763E-08</v>
       </c>
       <c r="B182">
-        <v>0.9992840205975387</v>
+        <v>0.9999999800175171</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183">
-        <v>0.07682293413743914</v>
+        <v>0.02828338590832817</v>
       </c>
       <c r="B183">
-        <v>0.923177065862561</v>
+        <v>0.9717166140916718</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184">
-        <v>0.02530090689484695</v>
+        <v>0.001184740763606561</v>
       </c>
       <c r="B184">
-        <v>0.974699093105153</v>
+        <v>0.9988152592363936</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185">
-        <v>0.3855827602345083</v>
+        <v>0.6639172618816821</v>
       </c>
       <c r="B185">
-        <v>0.6144172397654917</v>
+        <v>0.3360827381183179</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186">
-        <v>0.865978223994128</v>
+        <v>0.8190452504098501</v>
       </c>
       <c r="B186">
-        <v>0.134021776005872</v>
+        <v>0.1809547495901499</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187">
-        <v>0.8025081524037689</v>
+        <v>0.8328012859118299</v>
       </c>
       <c r="B187">
-        <v>0.1974918475962311</v>
+        <v>0.16719871408817</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188">
-        <v>0.0006951444195098928</v>
+        <v>3.124340547024155E-08</v>
       </c>
       <c r="B188">
-        <v>0.9993048555804903</v>
+        <v>0.9999999687565946</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189">
-        <v>0.0007256986106274195</v>
+        <v>6.943592520187815E-09</v>
       </c>
       <c r="B189">
-        <v>0.9992743013893726</v>
+        <v>0.9999999930564073</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190">
-        <v>0.002206727218176141</v>
+        <v>3.282482233600778E-08</v>
       </c>
       <c r="B190">
-        <v>0.9977932727818238</v>
+        <v>0.9999999671751776</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191">
-        <v>0.1614108645600766</v>
+        <v>0.0258976987606311</v>
       </c>
       <c r="B191">
-        <v>0.8385891354399233</v>
+        <v>0.974102301239369</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192">
-        <v>0.6983555732089353</v>
+        <v>0.8011560627224593</v>
       </c>
       <c r="B192">
-        <v>0.3016444267910646</v>
+        <v>0.1988439372775407</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193">
-        <v>0.587791588893381</v>
+        <v>0.810600226777527</v>
       </c>
       <c r="B193">
-        <v>0.412208411106619</v>
+        <v>0.1893997732224732</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194">
-        <v>0.1639323397512284</v>
+        <v>0.01829535079307684</v>
       </c>
       <c r="B194">
-        <v>0.8360676602487715</v>
+        <v>0.9817046492069231</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195">
-        <v>0.02999856674150664</v>
+        <v>0.01036288631229651</v>
       </c>
       <c r="B195">
-        <v>0.9700014332584934</v>
+        <v>0.9896371136877036</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196">
-        <v>0.02988291910763108</v>
+        <v>0.01506156631044707</v>
       </c>
       <c r="B196">
-        <v>0.9701170808923689</v>
+        <v>0.9849384336895531</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197">
-        <v>0.07437895804234428</v>
+        <v>0.00396644916456533</v>
       </c>
       <c r="B197">
-        <v>0.9256210419576558</v>
+        <v>0.9960335508354348</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198">
-        <v>0.7924479904943224</v>
+        <v>0.7975272236141699</v>
       </c>
       <c r="B198">
-        <v>0.2075520095056776</v>
+        <v>0.20247277638583</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199">
-        <v>0.05879737181749186</v>
+        <v>0.0107939563109994</v>
       </c>
       <c r="B199">
-        <v>0.941202628182508</v>
+        <v>0.9892060436890007</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200">
-        <v>0.00128795530507051</v>
+        <v>2.444156109226616E-07</v>
       </c>
       <c r="B200">
-        <v>0.9987120446949295</v>
+        <v>0.999999755584389</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201">
-        <v>0.5310101019015702</v>
+        <v>0.8178160568407917</v>
       </c>
       <c r="B201">
-        <v>0.4689898980984298</v>
+        <v>0.1821839431592083</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202">
-        <v>0.001204378723792924</v>
+        <v>1.482060551445502E-08</v>
       </c>
       <c r="B202">
-        <v>0.998795621276207</v>
+        <v>0.9999999851793944</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203">
-        <v>0.547567306808503</v>
+        <v>0.8245147398193171</v>
       </c>
       <c r="B203">
-        <v>0.4524326931914971</v>
+        <v>0.1754852601806829</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204">
-        <v>0.03186972703774048</v>
+        <v>1.245790354048634E-06</v>
       </c>
       <c r="B204">
-        <v>0.9681302729622596</v>
+        <v>0.999998754209646</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205">
-        <v>0.04448265378472557</v>
+        <v>0.00267929728222047</v>
       </c>
       <c r="B205">
-        <v>0.9555173462152745</v>
+        <v>0.9973207027177794</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206">
-        <v>0.004103261493127616</v>
+        <v>5.492754448882853E-07</v>
       </c>
       <c r="B206">
-        <v>0.9958967385068722</v>
+        <v>0.9999994507245552</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207">
-        <v>0.5677163018117927</v>
+        <v>0.7927655446549846</v>
       </c>
       <c r="B207">
-        <v>0.4322836981882074</v>
+        <v>0.2072344553450154</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208">
-        <v>0.2319591051325871</v>
+        <v>0.5965098280929191</v>
       </c>
       <c r="B208">
-        <v>0.768040894867413</v>
+        <v>0.4034901719070809</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209">
-        <v>0.03310664457957827</v>
+        <v>0.0002840776479684352</v>
       </c>
       <c r="B209">
-        <v>0.9668933554204217</v>
+        <v>0.9997159223520317</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210">
-        <v>0.7849143545690239</v>
+        <v>0.7885441051368418</v>
       </c>
       <c r="B210">
-        <v>0.215085645430976</v>
+        <v>0.2114558948631583</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211">
-        <v>0.03546088423326969</v>
+        <v>0.01492926515640861</v>
       </c>
       <c r="B211">
-        <v>0.9645391157667303</v>
+        <v>0.9850707348435914</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212">
-        <v>0.3781268142256137</v>
+        <v>0.7401137243387315</v>
       </c>
       <c r="B212">
-        <v>0.6218731857743863</v>
+        <v>0.2598862756612685</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213">
-        <v>0.006759644438415628</v>
+        <v>1.137792392619384E-07</v>
       </c>
       <c r="B213">
-        <v>0.9932403555615844</v>
+        <v>0.9999998862207607</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214">
-        <v>0.2637246128352573</v>
+        <v>0.7830899619636653</v>
       </c>
       <c r="B214">
-        <v>0.7362753871647425</v>
+        <v>0.2169100380363348</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215">
-        <v>0.05716591636885517</v>
+        <v>0.0142796619201675</v>
       </c>
       <c r="B215">
-        <v>0.9428340836311448</v>
+        <v>0.9857203380798325</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216">
-        <v>0.6265006461855501</v>
+        <v>0.8285027530877934</v>
       </c>
       <c r="B216">
-        <v>0.3734993538144499</v>
+        <v>0.1714972469122067</v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217">
-        <v>0.04483813388574306</v>
+        <v>0.01647515003030037</v>
       </c>
       <c r="B217">
-        <v>0.9551618661142569</v>
+        <v>0.9835248499696996</v>
       </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218">
-        <v>0.7170616902161489</v>
+        <v>0.7892359775226787</v>
       </c>
       <c r="B218">
-        <v>0.2829383097838512</v>
+        <v>0.2107640224773213</v>
       </c>
     </row>
     <row r="219" spans="1:2">
       <c r="A219">
-        <v>0.2553019378824931</v>
+        <v>0.6888177003920862</v>
       </c>
       <c r="B219">
-        <v>0.7446980621175069</v>
+        <v>0.3111822996079139</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220">
-        <v>0.4186789825774661</v>
+        <v>0.7099322729254287</v>
       </c>
       <c r="B220">
-        <v>0.5813210174225339</v>
+        <v>0.2900677270745712</v>
       </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221">
-        <v>0.9361899068855877</v>
+        <v>0.8307603692508284</v>
       </c>
       <c r="B221">
-        <v>0.0638100931144123</v>
+        <v>0.1692396307491717</v>
       </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222">
-        <v>0.6303320327131828</v>
+        <v>0.8040548424285788</v>
       </c>
       <c r="B222">
-        <v>0.3696679672868173</v>
+        <v>0.1959451575714212</v>
       </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223">
-        <v>0.114358218962745</v>
+        <v>0.0243084574389554</v>
       </c>
       <c r="B223">
-        <v>0.8856417810372552</v>
+        <v>0.9756915425610445</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224">
-        <v>0.7460113152061186</v>
+        <v>0.7812451067371289</v>
       </c>
       <c r="B224">
-        <v>0.2539886847938813</v>
+        <v>0.218754893262871</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225">
-        <v>0.2985843124687985</v>
+        <v>0.8091661182175186</v>
       </c>
       <c r="B225">
-        <v>0.7014156875312014</v>
+        <v>0.1908338817824815</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226">
-        <v>0.004528585433049044</v>
+        <v>3.225496014117402E-08</v>
       </c>
       <c r="B226">
-        <v>0.9954714145669509</v>
+        <v>0.9999999677450397</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227">
-        <v>0.1022025203038001</v>
+        <v>0.02171503626136178</v>
       </c>
       <c r="B227">
-        <v>0.8977974796961998</v>
+        <v>0.9782849637386382</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228">
-        <v>0.2559287295659594</v>
+        <v>0.6837794840237735</v>
       </c>
       <c r="B228">
-        <v>0.7440712704340405</v>
+        <v>0.3162205159762264</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229">
-        <v>0.053119579665535</v>
+        <v>0.01688255062357166</v>
       </c>
       <c r="B229">
-        <v>0.946880420334465</v>
+        <v>0.9831174493764286</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230">
-        <v>0.7533854276692715</v>
+        <v>0.8061694201223779</v>
       </c>
       <c r="B230">
-        <v>0.2466145723307285</v>
+        <v>0.1938305798776222</v>
       </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231">
-        <v>0.3548293578798778</v>
+        <v>0.6377185785868194</v>
       </c>
       <c r="B231">
-        <v>0.6451706421201222</v>
+        <v>0.3622814214131806</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232">
-        <v>0.3077035675699333</v>
+        <v>0.7605996581529234</v>
       </c>
       <c r="B232">
-        <v>0.6922964324300668</v>
+        <v>0.2394003418470765</v>
       </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233">
-        <v>0.0006635366942324102</v>
+        <v>9.155019365793492E-09</v>
       </c>
       <c r="B233">
-        <v>0.9993364633057674</v>
+        <v>0.9999999908449806</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234">
-        <v>0.6565859776670032</v>
+        <v>0.807273739976159</v>
       </c>
       <c r="B234">
-        <v>0.3434140223329969</v>
+        <v>0.1927262600238407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>